<commit_message>
working version with JSON Stubbs
</commit_message>
<xml_diff>
--- a/iglCLI/test.xlsx
+++ b/iglCLI/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23715" windowHeight="11145" xr2:uid="{2FDD33C0-A038-476C-9DD5-35A214C0D2B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23717" windowHeight="11143" xr2:uid="{2FDD33C0-A038-476C-9DD5-35A214C0D2B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2118,13 +2117,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0D0B00-7E91-409F-99C1-CAC1CD6FA046}">
   <dimension ref="C6:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C7">
         <v>1</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C8">
         <v>2</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C9">
         <v>3</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C10">
         <v>4</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C11">
         <v>5</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C12">
         <v>6</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C13">
         <v>7</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C14">
         <v>8</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C15">
         <v>9</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.4">
       <c r="C16">
         <v>10</v>
       </c>

</xml_diff>